<commit_message>
Ajout de la feuille de mesure
</commit_message>
<xml_diff>
--- a/Metrics_sheet.xlsx
+++ b/Metrics_sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/sandiaye_unicef_org/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="320" documentId="8_{48645364-D1C8-4FEB-9C6A-56557003A6A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C4897F8F-BCE1-40AE-9E88-EB0444CBD349}"/>
+  <xr:revisionPtr revIDLastSave="335" documentId="8_{48645364-D1C8-4FEB-9C6A-56557003A6A4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{FDCD953D-A7AF-4671-8978-D6A97BC7E569}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{99FE6BB3-69C2-2E48-9360-61301171499D}"/>
   </bookViews>
@@ -105,7 +105,7 @@
     <t>Type de rapportage du mois</t>
   </si>
   <si>
-    <t xml:space="preserve">Définit si les données envoyées sont un rapport ou un rapport de rappel </t>
+    <t xml:space="preserve">Définit si les données envoyées sont un rapport, un retard de rapport ou un rapport de rappel </t>
   </si>
   <si>
     <t>Mensuel</t>
@@ -117,7 +117,7 @@
     <t>Nombre de rapport mensuel par agent</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre de rapport </t>
+    <t xml:space="preserve">Nombre de rapports </t>
   </si>
   <si>
     <t xml:space="preserve">Comparaison(date_rapport(le mois), mois_de_rapport) </t>
@@ -132,7 +132,7 @@
     <t>Nombre de rapports de rappel</t>
   </si>
   <si>
-    <t xml:space="preserve"> Comparaison(date_rapport_de_rappel(le mois) &amp; mois_de_rapport)</t>
+    <t xml:space="preserve"> Comparaison(date_rapport_de_rappel(le mois) &amp; mois_de_rapport) &amp;&amp; Comparaison(date_rapport_de_rappel(l'année) &amp; annee_en_cours)</t>
   </si>
   <si>
     <t>Département, Annee, Commune</t>
@@ -150,10 +150,10 @@
     <t>Année</t>
   </si>
   <si>
-    <t>Nombre des agents ayant délivrés 12 rapports</t>
-  </si>
-  <si>
-    <t>Calcule le nombre des agents ayant complétés les 12 rapports de l'année</t>
+    <t>Nombre des agents assidus</t>
+  </si>
+  <si>
+    <t>Calcule le nombre de rapports total délivrés par les agents du début de l'année jusqu'au mois en cours</t>
   </si>
   <si>
     <t xml:space="preserve">somme des rapports + somme des rapports de rappel </t>
@@ -168,7 +168,7 @@
     <t>Nombre de jours ecoulés avant que le contact n'envoie son rapport mensuel</t>
   </si>
   <si>
-    <t>date_rapport - 1er jour mois_de_rapport</t>
+    <t>date_rapport - 1er jour succédant le mois_de_rapport</t>
   </si>
   <si>
     <t>Temps moyen de rapportage de l'agent dans l'année</t>
@@ -199,7 +199,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -602,26 +602,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5072CAA1-CFBB-894A-ABE2-2048B0CBA7E5}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="174" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.58203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.08203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.58203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="50.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="28.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="24.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="44.1" thickBot="1">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -650,7 +650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="47.1" thickTop="1">
+    <row r="2" spans="1:9" ht="47" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -670,7 +670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30.95">
+    <row r="3" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -687,7 +687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30.95">
+    <row r="4" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -707,7 +707,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30.95">
+    <row r="5" spans="1:9" ht="62" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -727,7 +727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="47.25">
+    <row r="6" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -747,7 +747,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30.95">
+    <row r="7" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -767,7 +767,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="46.5">
+    <row r="8" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -787,7 +787,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="46.5">
+    <row r="9" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -804,7 +804,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="46.5">
+    <row r="10" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -821,7 +821,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="46.5">
+    <row r="11" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -848,6 +848,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED7C61AFC03BC44091C5B9D71DA1CB22" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff0fcc5f519ba2dee47963f00d22da3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb14854c-05ba-4eae-ae54-68d5e6f8c49b" xmlns:ns4="c1e561a4-e13e-4d4b-a29f-9d5871c8a3c9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="736222a4900a1aaa6fbd5fd8b093b4e8" ns3:_="" ns4:_="">
     <xsd:import namespace="fb14854c-05ba-4eae-ae54-68d5e6f8c49b"/>
@@ -1044,15 +1053,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1060,13 +1060,45 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39158A6D-D005-41BB-BB33-C27E61C9FC44}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937CA4CB-6CCB-426B-A8E9-FB7243F4EC04}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937CA4CB-6CCB-426B-A8E9-FB7243F4EC04}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39158A6D-D005-41BB-BB33-C27E61C9FC44}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fb14854c-05ba-4eae-ae54-68d5e6f8c49b"/>
+    <ds:schemaRef ds:uri="c1e561a4-e13e-4d4b-a29f-9d5871c8a3c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD504793-B749-4EA4-BC70-1195B8C10BDB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD504793-B749-4EA4-BC70-1195B8C10BDB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fb14854c-05ba-4eae-ae54-68d5e6f8c49b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c1e561a4-e13e-4d4b-a29f-9d5871c8a3c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>